<commit_message>
creating RMD for objectives one and two
</commit_message>
<xml_diff>
--- a/Data_extraction_postcrosschecking.xlsx
+++ b/Data_extraction_postcrosschecking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z3439723_ad_unsw_edu_au/Documents/Overview of reviews_trans environment effects/Analysis/Nongen_map_of_reviews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C8DE252-67D3-437E-999F-0322730C74C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{5C8DE252-67D3-437E-999F-0322730C74C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{847C55FD-3F09-474C-8DF1-FF723277AB8E}"/>
   <bookViews>
-    <workbookView xWindow="-29850" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="9" activeTab="14" xr2:uid="{E4D07577-1050-462D-A7B0-049CD472D6CE}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="5" xr2:uid="{E4D07577-1050-462D-A7B0-049CD472D6CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Publication_info" sheetId="1" r:id="rId1"/>
@@ -3981,8 +3981,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B06098-F9D7-4E2C-96DC-A163CE4FD1C7}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10356,7 +10359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9733E463-A3C7-4753-9858-703C94BFFF08}">
   <dimension ref="A1:AH60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -14561,8 +14564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B936721-69C3-4A8C-8098-3E46F9E5D7C2}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14598,53 +14601,53 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>298</v>
       </c>
+      <c r="C2" t="s">
+        <v>309</v>
+      </c>
       <c r="D2" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="F2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H2" t="s">
         <v>300</v>
-      </c>
-      <c r="H2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
         <v>298</v>
       </c>
       <c r="D3" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="F3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" t="s">
+        <v>330</v>
+      </c>
+      <c r="H3" t="s">
         <v>300</v>
-      </c>
-      <c r="G3" t="s">
-        <v>302</v>
-      </c>
-      <c r="H3" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>278</v>
-      </c>
-      <c r="C4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D4" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="F4" t="s">
         <v>304</v>
@@ -14655,19 +14658,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s">
-        <v>305</v>
-      </c>
-      <c r="C5" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D5" t="s">
         <v>307</v>
       </c>
       <c r="F5" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="H5" t="s">
         <v>300</v>
@@ -14675,10 +14675,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>236</v>
       </c>
       <c r="B6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D6" t="s">
         <v>307</v>
@@ -14692,53 +14692,56 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D7" t="s">
-        <v>307</v>
+        <v>312</v>
+      </c>
+      <c r="E7" t="s">
+        <v>327</v>
       </c>
       <c r="F7" t="s">
         <v>301</v>
       </c>
       <c r="H7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D8" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F8" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>278</v>
-      </c>
-      <c r="C9" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="D9" t="s">
         <v>299</v>
       </c>
       <c r="F9" t="s">
-        <v>304</v>
+        <v>300</v>
+      </c>
+      <c r="G9" t="s">
+        <v>302</v>
       </c>
       <c r="H9" t="s">
         <v>278</v>
@@ -14746,30 +14749,33 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D10" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F10" t="s">
         <v>304</v>
       </c>
       <c r="H10" t="s">
-        <v>300</v>
+        <v>278</v>
+      </c>
+      <c r="I10" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>213</v>
       </c>
       <c r="B11" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D11" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F11" t="s">
         <v>304</v>
@@ -14780,16 +14786,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>249</v>
       </c>
       <c r="B12" t="s">
         <v>298</v>
       </c>
-      <c r="C12" t="s">
-        <v>309</v>
-      </c>
       <c r="D12" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="F12" t="s">
         <v>304</v>
@@ -14800,28 +14803,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>257</v>
       </c>
       <c r="B13" t="s">
+        <v>298</v>
+      </c>
+      <c r="D13" t="s">
+        <v>320</v>
+      </c>
+      <c r="F13" t="s">
         <v>278</v>
       </c>
-      <c r="C13" t="s">
-        <v>311</v>
-      </c>
-      <c r="D13" t="s">
-        <v>312</v>
-      </c>
-      <c r="E13" t="s">
-        <v>313</v>
-      </c>
-      <c r="F13" t="s">
-        <v>304</v>
-      </c>
       <c r="G13" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="H13" t="s">
-        <v>300</v>
+        <v>278</v>
+      </c>
+      <c r="I13" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -14843,16 +14843,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>279</v>
       </c>
       <c r="B15" t="s">
         <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E15" t="s">
-        <v>315</v>
+        <v>342</v>
       </c>
       <c r="F15" t="s">
         <v>304</v>
@@ -14863,13 +14863,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>286</v>
       </c>
       <c r="B16" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="D16" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="F16" t="s">
         <v>304</v>
@@ -14880,16 +14880,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
         <v>305</v>
       </c>
+      <c r="C17" t="s">
+        <v>306</v>
+      </c>
       <c r="D17" t="s">
         <v>307</v>
       </c>
       <c r="F17" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H17" t="s">
         <v>300</v>
@@ -14897,7 +14900,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>305</v>
@@ -14914,36 +14917,30 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="D19" t="s">
         <v>307</v>
       </c>
       <c r="F19" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H19" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>278</v>
-      </c>
-      <c r="C20" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="D20" t="s">
-        <v>278</v>
-      </c>
-      <c r="E20" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="F20" t="s">
         <v>304</v>
@@ -14954,79 +14951,64 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="D21" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="F21" t="s">
         <v>304</v>
       </c>
       <c r="H21" t="s">
-        <v>278</v>
-      </c>
-      <c r="I21" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="D22" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="F22" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H22" t="s">
         <v>300</v>
       </c>
-      <c r="I22" t="s">
-        <v>319</v>
-      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
         <v>305</v>
       </c>
       <c r="D23" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="F23" t="s">
         <v>304</v>
       </c>
       <c r="H23" t="s">
-        <v>278</v>
-      </c>
-      <c r="I23" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>278</v>
-      </c>
-      <c r="C24" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="D24" t="s">
-        <v>310</v>
-      </c>
-      <c r="E24" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="F24" t="s">
         <v>304</v>
@@ -15037,82 +15019,73 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B25" t="s">
         <v>305</v>
       </c>
       <c r="D25" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="F25" t="s">
         <v>304</v>
       </c>
       <c r="H25" t="s">
-        <v>301</v>
-      </c>
-      <c r="I25" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="B26" t="s">
         <v>305</v>
       </c>
       <c r="D26" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="F26" t="s">
         <v>304</v>
       </c>
+      <c r="G26" t="s">
+        <v>331</v>
+      </c>
       <c r="H26" t="s">
-        <v>301</v>
-      </c>
-      <c r="I26" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s">
-        <v>278</v>
-      </c>
-      <c r="C27" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="D27" t="s">
-        <v>278</v>
-      </c>
-      <c r="E27" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="F27" t="s">
         <v>304</v>
       </c>
       <c r="H27" t="s">
-        <v>300</v>
+        <v>278</v>
+      </c>
+      <c r="I27" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="B28" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="D28" t="s">
-        <v>312</v>
-      </c>
-      <c r="E28" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="F28" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H28" t="s">
         <v>300</v>
@@ -15120,7 +15093,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>164</v>
+        <v>217</v>
       </c>
       <c r="B29" t="s">
         <v>305</v>
@@ -15137,19 +15110,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>221</v>
       </c>
       <c r="B30" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="D30" t="s">
-        <v>278</v>
+        <v>307</v>
       </c>
       <c r="F30" t="s">
-        <v>300</v>
-      </c>
-      <c r="G30" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="H30" t="s">
         <v>300</v>
@@ -15157,19 +15127,19 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>234</v>
       </c>
       <c r="B31" t="s">
         <v>305</v>
       </c>
       <c r="D31" t="s">
-        <v>278</v>
-      </c>
-      <c r="E31" t="s">
-        <v>329</v>
+        <v>307</v>
       </c>
       <c r="F31" t="s">
-        <v>304</v>
+        <v>300</v>
+      </c>
+      <c r="G31" t="s">
+        <v>336</v>
       </c>
       <c r="H31" t="s">
         <v>300</v>
@@ -15177,19 +15147,16 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="B32" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="D32" t="s">
         <v>307</v>
       </c>
       <c r="F32" t="s">
-        <v>278</v>
-      </c>
-      <c r="G32" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="H32" t="s">
         <v>300</v>
@@ -15197,10 +15164,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>247</v>
       </c>
       <c r="B33" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="D33" t="s">
         <v>307</v>
@@ -15214,7 +15181,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>186</v>
+        <v>252</v>
       </c>
       <c r="B34" t="s">
         <v>305</v>
@@ -15225,22 +15192,19 @@
       <c r="F34" t="s">
         <v>304</v>
       </c>
-      <c r="G34" t="s">
-        <v>331</v>
-      </c>
       <c r="H34" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>262</v>
       </c>
       <c r="B35" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="D35" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F35" t="s">
         <v>304</v>
@@ -15251,7 +15215,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>193</v>
+        <v>264</v>
       </c>
       <c r="B36" t="s">
         <v>305</v>
@@ -15260,27 +15224,27 @@
         <v>307</v>
       </c>
       <c r="F36" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H36" t="s">
         <v>278</v>
       </c>
       <c r="I36" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>267</v>
       </c>
       <c r="B37" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="D37" t="s">
         <v>307</v>
       </c>
       <c r="F37" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="H37" t="s">
         <v>300</v>
@@ -15288,7 +15252,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>204</v>
+        <v>269</v>
       </c>
       <c r="B38" t="s">
         <v>305</v>
@@ -15305,36 +15269,36 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>208</v>
+        <v>275</v>
       </c>
       <c r="B39" t="s">
         <v>305</v>
       </c>
       <c r="D39" t="s">
-        <v>312</v>
-      </c>
-      <c r="E39" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="F39" t="s">
-        <v>304</v>
+        <v>301</v>
+      </c>
+      <c r="G39" t="s">
+        <v>341</v>
       </c>
       <c r="H39" t="s">
-        <v>278</v>
-      </c>
-      <c r="I39" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>213</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="D40" t="s">
-        <v>299</v>
+        <v>312</v>
+      </c>
+      <c r="E40" t="s">
+        <v>315</v>
       </c>
       <c r="F40" t="s">
         <v>304</v>
@@ -15345,41 +15309,50 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B41" t="s">
         <v>305</v>
       </c>
       <c r="D41" t="s">
-        <v>307</v>
+        <v>312</v>
+      </c>
+      <c r="E41" t="s">
+        <v>333</v>
       </c>
       <c r="F41" t="s">
         <v>304</v>
       </c>
       <c r="H41" t="s">
-        <v>300</v>
+        <v>278</v>
+      </c>
+      <c r="I41" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>221</v>
+        <v>136</v>
       </c>
       <c r="B42" t="s">
         <v>305</v>
       </c>
       <c r="D42" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="F42" t="s">
         <v>304</v>
       </c>
       <c r="H42" t="s">
-        <v>300</v>
+        <v>278</v>
+      </c>
+      <c r="I42" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>225</v>
+        <v>147</v>
       </c>
       <c r="B43" t="s">
         <v>305</v>
@@ -15394,12 +15367,12 @@
         <v>301</v>
       </c>
       <c r="I43" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>229</v>
+        <v>151</v>
       </c>
       <c r="B44" t="s">
         <v>305</v>
@@ -15411,38 +15384,41 @@
         <v>304</v>
       </c>
       <c r="H44" t="s">
-        <v>300</v>
+        <v>301</v>
+      </c>
+      <c r="I44" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B45" t="s">
         <v>305</v>
       </c>
       <c r="D45" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="F45" t="s">
-        <v>300</v>
-      </c>
-      <c r="G45" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="H45" t="s">
-        <v>300</v>
+        <v>301</v>
+      </c>
+      <c r="I45" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B46" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="D46" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="F46" t="s">
         <v>304</v>
@@ -15453,34 +15429,37 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>239</v>
+        <v>283</v>
       </c>
       <c r="B47" t="s">
         <v>305</v>
       </c>
       <c r="D47" t="s">
-        <v>307</v>
+        <v>320</v>
       </c>
       <c r="F47" t="s">
         <v>304</v>
       </c>
       <c r="H47" t="s">
-        <v>300</v>
+        <v>278</v>
+      </c>
+      <c r="I47" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>243</v>
+        <v>175</v>
       </c>
       <c r="B48" t="s">
-        <v>278</v>
-      </c>
-      <c r="C48" t="s">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="D48" t="s">
         <v>307</v>
       </c>
+      <c r="E48" t="s">
+        <v>329</v>
+      </c>
       <c r="F48" t="s">
         <v>304</v>
       </c>
@@ -15490,13 +15469,19 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>247</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
-        <v>305</v>
+        <v>278</v>
+      </c>
+      <c r="C49" t="s">
+        <v>322</v>
       </c>
       <c r="D49" t="s">
-        <v>307</v>
+        <v>310</v>
+      </c>
+      <c r="E49" t="s">
+        <v>323</v>
       </c>
       <c r="F49" t="s">
         <v>304</v>
@@ -15507,13 +15492,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>249</v>
+        <v>190</v>
       </c>
       <c r="B50" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="D50" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="F50" t="s">
         <v>304</v>
@@ -15524,10 +15509,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>252</v>
+        <v>116</v>
       </c>
       <c r="B51" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="D51" t="s">
         <v>307</v>
@@ -15541,90 +15526,99 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="B52" t="s">
-        <v>298</v>
+        <v>278</v>
+      </c>
+      <c r="C52" t="s">
+        <v>337</v>
       </c>
       <c r="D52" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="F52" t="s">
-        <v>278</v>
-      </c>
-      <c r="G52" t="s">
-        <v>338</v>
+        <v>304</v>
       </c>
       <c r="H52" t="s">
-        <v>278</v>
-      </c>
-      <c r="I52" t="s">
-        <v>339</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>262</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>305</v>
+        <v>278</v>
+      </c>
+      <c r="C53" t="s">
+        <v>311</v>
       </c>
       <c r="D53" t="s">
-        <v>307</v>
+        <v>312</v>
+      </c>
+      <c r="E53" t="s">
+        <v>313</v>
       </c>
       <c r="F53" t="s">
         <v>304</v>
       </c>
+      <c r="G53" t="s">
+        <v>314</v>
+      </c>
       <c r="H53" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>264</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>305</v>
+        <v>278</v>
+      </c>
+      <c r="C54" t="s">
+        <v>303</v>
       </c>
       <c r="D54" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F54" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H54" t="s">
-        <v>278</v>
-      </c>
-      <c r="I54" t="s">
-        <v>340</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>267</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>305</v>
+        <v>278</v>
+      </c>
+      <c r="C55" t="s">
+        <v>308</v>
       </c>
       <c r="D55" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F55" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H55" t="s">
-        <v>300</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>269</v>
+        <v>98</v>
       </c>
       <c r="B56" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="D56" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F56" t="s">
         <v>304</v>
@@ -15635,36 +15629,39 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>275</v>
+        <v>131</v>
       </c>
       <c r="B57" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="D57" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F57" t="s">
         <v>301</v>
       </c>
-      <c r="G57" t="s">
-        <v>341</v>
-      </c>
       <c r="H57" t="s">
         <v>300</v>
       </c>
+      <c r="I57" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>279</v>
+        <v>122</v>
       </c>
       <c r="B58" t="s">
-        <v>305</v>
+        <v>278</v>
+      </c>
+      <c r="C58" t="s">
+        <v>316</v>
       </c>
       <c r="D58" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E58" t="s">
-        <v>342</v>
+        <v>317</v>
       </c>
       <c r="F58" t="s">
         <v>304</v>
@@ -15675,42 +15672,51 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>283</v>
+        <v>156</v>
       </c>
       <c r="B59" t="s">
-        <v>305</v>
+        <v>278</v>
+      </c>
+      <c r="C59" t="s">
+        <v>325</v>
       </c>
       <c r="D59" t="s">
-        <v>320</v>
+        <v>299</v>
+      </c>
+      <c r="E59" t="s">
+        <v>326</v>
       </c>
       <c r="F59" t="s">
         <v>304</v>
       </c>
       <c r="H59" t="s">
-        <v>278</v>
-      </c>
-      <c r="I59" t="s">
-        <v>340</v>
+        <v>300</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>286</v>
+        <v>169</v>
       </c>
       <c r="B60" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="D60" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="F60" t="s">
-        <v>304</v>
+        <v>300</v>
+      </c>
+      <c r="G60" t="s">
+        <v>328</v>
       </c>
       <c r="H60" t="s">
         <v>300</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I60">
+    <sortCondition ref="B2:B60"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{71E7C872-908C-4119-BF8C-8CEDAA69FF3A}">
@@ -16397,8 +16403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61DB050-FA39-425C-8BE9-84756207D428}">
   <dimension ref="A1:C561"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A452" workbookViewId="0">
+      <selection activeCell="A561" sqref="A561:XFD561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21284,8 +21290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55DD04B-0525-4DE5-97CF-5C1840F71413}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21315,34 +21321,31 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>278</v>
-      </c>
-      <c r="C5" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>651</v>
@@ -21350,7 +21353,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>651</v>
@@ -21358,7 +21361,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>651</v>
@@ -21366,7 +21369,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>651</v>
@@ -21374,15 +21377,15 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
         <v>651</v>
@@ -21390,15 +21393,18 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
         <v>651</v>
       </c>
+      <c r="C12" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
         <v>651</v>
@@ -21406,7 +21412,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
         <v>651</v>
@@ -21414,7 +21420,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
         <v>651</v>
@@ -21422,26 +21428,23 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
         <v>651</v>
       </c>
-      <c r="C16" t="s">
-        <v>655</v>
-      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
         <v>651</v>
@@ -21449,7 +21452,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
         <v>651</v>
@@ -21457,7 +21460,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
         <v>651</v>
@@ -21465,7 +21468,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
         <v>651</v>
@@ -21473,7 +21476,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
         <v>651</v>
@@ -21481,7 +21484,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="B23" t="s">
         <v>651</v>
@@ -21489,15 +21492,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
         <v>651</v>
       </c>
+      <c r="C24" t="s">
+        <v>656</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>585</v>
       </c>
       <c r="B25" t="s">
         <v>651</v>
@@ -21505,7 +21511,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="B26" t="s">
         <v>651</v>
@@ -21513,23 +21519,26 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="B27" t="s">
-        <v>652</v>
+        <v>651</v>
+      </c>
+      <c r="C27" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="B28" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
         <v>651</v>
@@ -21537,7 +21546,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
         <v>651</v>
@@ -21545,318 +21554,318 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="B31" t="s">
         <v>651</v>
       </c>
-      <c r="C31" t="s">
-        <v>656</v>
-      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>585</v>
+        <v>186</v>
       </c>
       <c r="B32" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>190</v>
       </c>
       <c r="B33" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="B34" t="s">
         <v>651</v>
       </c>
-      <c r="C34" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
       <c r="B35" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="B36" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="B37" t="s">
-        <v>652</v>
-      </c>
-      <c r="C37" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="B38" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>179</v>
+        <v>225</v>
       </c>
       <c r="B39" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="B40" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>186</v>
+        <v>234</v>
       </c>
       <c r="B41" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="B42" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>193</v>
+        <v>239</v>
       </c>
       <c r="B43" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="B44" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>204</v>
+        <v>247</v>
       </c>
       <c r="B45" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>208</v>
+        <v>252</v>
       </c>
       <c r="B46" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>213</v>
+        <v>262</v>
       </c>
       <c r="B47" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="B48" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>221</v>
+        <v>269</v>
       </c>
       <c r="B49" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="B50" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>229</v>
+        <v>279</v>
       </c>
       <c r="B51" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>234</v>
+        <v>283</v>
       </c>
       <c r="B52" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>236</v>
+        <v>286</v>
       </c>
       <c r="B53" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>239</v>
+        <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>243</v>
+        <v>131</v>
       </c>
       <c r="B55" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
       <c r="B56" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>249</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>252</v>
+        <v>42</v>
       </c>
       <c r="B58" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>257</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>264</v>
+        <v>169</v>
       </c>
       <c r="B61" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>267</v>
+        <v>198</v>
       </c>
       <c r="B62" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>267</v>
+        <v>204</v>
       </c>
       <c r="B63" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B64" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B65" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>279</v>
+        <v>19</v>
       </c>
       <c r="B66" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="C66" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="B67" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>286</v>
+        <v>257</v>
       </c>
       <c r="B68" t="s">
-        <v>651</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C68">
+    <sortCondition ref="B2:B68"/>
+  </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{56FA97DB-1440-4EC5-B2A1-CACE9C0A9039}">
       <formula1>"matriline, patriline, not separated, unclear"</formula1>
@@ -22474,8 +22483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2AD6296-90D1-4756-8186-5D60BB2CB704}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22505,15 +22514,15 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>668</v>
@@ -22521,7 +22530,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>668</v>
@@ -22529,7 +22538,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
         <v>668</v>
@@ -22537,7 +22546,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>668</v>
@@ -22545,34 +22554,40 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>669</v>
+        <v>668</v>
+      </c>
+      <c r="C8" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>668</v>
       </c>
+      <c r="C9" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
         <v>668</v>
       </c>
       <c r="C10" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
         <v>668</v>
@@ -22583,37 +22598,31 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
         <v>668</v>
       </c>
-      <c r="C12" t="s">
-        <v>671</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
         <v>668</v>
       </c>
-      <c r="C13" t="s">
-        <v>671</v>
-      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
         <v>668</v>
@@ -22621,7 +22630,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
         <v>668</v>
@@ -22629,7 +22638,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
         <v>668</v>
@@ -22637,7 +22646,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
         <v>668</v>
@@ -22645,7 +22654,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
         <v>668</v>
@@ -22653,7 +22662,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
         <v>668</v>
@@ -22661,7 +22670,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
         <v>668</v>
@@ -22669,7 +22678,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
         <v>668</v>
@@ -22677,7 +22686,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
         <v>668</v>
@@ -22685,15 +22694,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>585</v>
       </c>
       <c r="B24" t="s">
-        <v>669</v>
+        <v>668</v>
+      </c>
+      <c r="C24" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="B25" t="s">
         <v>668</v>
@@ -22701,7 +22713,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B26" t="s">
         <v>668</v>
@@ -22709,7 +22721,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B27" t="s">
         <v>668</v>
@@ -22717,18 +22729,15 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>585</v>
+        <v>169</v>
       </c>
       <c r="B28" t="s">
         <v>668</v>
       </c>
-      <c r="C28" t="s">
-        <v>672</v>
-      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
         <v>668</v>
@@ -22736,15 +22745,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
         <v>668</v>
       </c>
+      <c r="C30" t="s">
+        <v>672</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="B31" t="s">
         <v>668</v>
@@ -22752,7 +22764,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="B32" t="s">
         <v>668</v>
@@ -22760,7 +22772,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="B33" t="s">
         <v>668</v>
@@ -22768,18 +22780,15 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B34" t="s">
         <v>668</v>
       </c>
-      <c r="C34" t="s">
-        <v>672</v>
-      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="B35" t="s">
         <v>668</v>
@@ -22787,7 +22796,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="B36" t="s">
         <v>668</v>
@@ -22795,7 +22804,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="B37" t="s">
         <v>668</v>
@@ -22803,7 +22812,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="B38" t="s">
         <v>668</v>
@@ -22811,7 +22820,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="B39" t="s">
         <v>668</v>
@@ -22819,15 +22828,18 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="B40" t="s">
         <v>668</v>
       </c>
+      <c r="C40" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="B41" t="s">
         <v>668</v>
@@ -22835,7 +22847,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="B42" t="s">
         <v>668</v>
@@ -22843,7 +22855,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="B43" t="s">
         <v>668</v>
@@ -22851,18 +22863,15 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="B44" t="s">
         <v>668</v>
       </c>
-      <c r="C44" t="s">
-        <v>673</v>
-      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="B45" t="s">
         <v>668</v>
@@ -22870,7 +22879,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B46" t="s">
         <v>668</v>
@@ -22878,7 +22887,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="B47" t="s">
         <v>668</v>
@@ -22886,15 +22895,18 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="B48" t="s">
         <v>668</v>
       </c>
+      <c r="C48" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="B49" t="s">
         <v>668</v>
@@ -22902,7 +22914,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="B50" t="s">
         <v>668</v>
@@ -22910,7 +22922,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="B51" t="s">
         <v>668</v>
@@ -22918,18 +22930,18 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="B52" t="s">
         <v>668</v>
       </c>
       <c r="C52" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="B53" t="s">
         <v>668</v>
@@ -22937,7 +22949,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="B54" t="s">
         <v>668</v>
@@ -22945,18 +22957,18 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="B55" t="s">
-        <v>278</v>
+        <v>668</v>
       </c>
       <c r="C55" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="B56" t="s">
         <v>668</v>
@@ -22964,18 +22976,18 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="B57" t="s">
         <v>668</v>
       </c>
       <c r="C57" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>264</v>
+        <v>13</v>
       </c>
       <c r="B58" t="s">
         <v>669</v>
@@ -22983,7 +22995,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>267</v>
+        <v>42</v>
       </c>
       <c r="B59" t="s">
         <v>669</v>
@@ -22991,51 +23003,51 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>269</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>275</v>
+        <v>131</v>
       </c>
       <c r="B61" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="B62" t="s">
-        <v>668</v>
-      </c>
-      <c r="C62" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="B63" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>286</v>
+        <v>257</v>
       </c>
       <c r="B64" t="s">
-        <v>668</v>
+        <v>278</v>
       </c>
       <c r="C64" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C64">
+    <sortCondition ref="B2:B64"/>
+  </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{79F80A56-918F-4653-9791-DE5550ECDD9E}">
       <formula1>"inter, trans, unclear"</formula1>
@@ -23050,7 +23062,7 @@
   <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G1048576"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23080,55 +23092,64 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
         <v>680</v>
       </c>
+      <c r="C4" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
-        <v>681</v>
+        <v>680</v>
+      </c>
+      <c r="C7" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>267</v>
       </c>
       <c r="B8" t="s">
-        <v>681</v>
+        <v>680</v>
+      </c>
+      <c r="C8" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>681</v>
@@ -23136,7 +23157,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>681</v>
@@ -23144,15 +23165,15 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
         <v>681</v>
@@ -23160,153 +23181,147 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B17" t="s">
-        <v>278</v>
+        <v>681</v>
+      </c>
+      <c r="C17" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
         <v>681</v>
       </c>
-      <c r="C18" t="s">
-        <v>682</v>
-      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>208</v>
       </c>
       <c r="B21" t="s">
-        <v>278</v>
-      </c>
-      <c r="C21" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="B22" t="s">
-        <v>278</v>
+        <v>681</v>
       </c>
       <c r="C22" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>247</v>
       </c>
       <c r="B23" t="s">
-        <v>680</v>
-      </c>
-      <c r="C23" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>262</v>
       </c>
       <c r="B24" t="s">
         <v>681</v>
       </c>
+      <c r="C24" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>267</v>
       </c>
       <c r="B25" t="s">
-        <v>680</v>
+        <v>681</v>
+      </c>
+      <c r="C25" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>681</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
         <v>278</v>
       </c>
-      <c r="C27" t="s">
-        <v>686</v>
-      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
         <v>278</v>
       </c>
-      <c r="C28" t="s">
-        <v>687</v>
-      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
         <v>278</v>
@@ -23314,7 +23329,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>585</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
         <v>278</v>
@@ -23322,18 +23337,15 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
         <v>278</v>
       </c>
-      <c r="C31" t="s">
-        <v>688</v>
-      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
         <v>278</v>
@@ -23341,7 +23353,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
         <v>278</v>
@@ -23349,39 +23361,51 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>680</v>
+        <v>278</v>
+      </c>
+      <c r="C34" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>681</v>
+        <v>278</v>
+      </c>
+      <c r="C35" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
         <v>278</v>
       </c>
+      <c r="C36" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
       <c r="B37" t="s">
         <v>278</v>
       </c>
+      <c r="C37" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
         <v>278</v>
@@ -23389,29 +23413,26 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>186</v>
+        <v>585</v>
       </c>
       <c r="B39" t="s">
         <v>278</v>
       </c>
-      <c r="C39" t="s">
-        <v>689</v>
-      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="B40" t="s">
         <v>278</v>
       </c>
       <c r="C40" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
       <c r="B41" t="s">
         <v>278</v>
@@ -23419,18 +23440,15 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="B42" t="s">
         <v>278</v>
       </c>
-      <c r="C42" t="s">
-        <v>683</v>
-      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="B43" t="s">
         <v>278</v>
@@ -23438,45 +23456,45 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
       <c r="B44" t="s">
-        <v>680</v>
-      </c>
-      <c r="C44" t="s">
-        <v>690</v>
+        <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="B45" t="s">
-        <v>681</v>
+        <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="B46" t="s">
         <v>278</v>
       </c>
+      <c r="C46" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="B47" t="s">
         <v>278</v>
       </c>
       <c r="C47" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="B48" t="s">
         <v>278</v>
@@ -23484,15 +23502,18 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="B49" t="s">
         <v>278</v>
       </c>
+      <c r="C49" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="B50" t="s">
         <v>278</v>
@@ -23500,26 +23521,26 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="B51" t="s">
-        <v>681</v>
-      </c>
-      <c r="C51" t="s">
-        <v>692</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="B52" t="s">
         <v>278</v>
       </c>
+      <c r="C52" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="B53" t="s">
         <v>278</v>
@@ -23527,7 +23548,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="B54" t="s">
         <v>278</v>
@@ -23535,15 +23556,15 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="B55" t="s">
-        <v>681</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="B56" t="s">
         <v>278</v>
@@ -23551,7 +23572,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B57" t="s">
         <v>278</v>
@@ -23559,7 +23580,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="B58" t="s">
         <v>278</v>
@@ -23567,18 +23588,15 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="B59" t="s">
-        <v>681</v>
-      </c>
-      <c r="C59" t="s">
-        <v>693</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="B60" t="s">
         <v>278</v>
@@ -23586,24 +23604,18 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B61" t="s">
-        <v>680</v>
-      </c>
-      <c r="C61" t="s">
-        <v>694</v>
+        <v>278</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B62" t="s">
-        <v>681</v>
-      </c>
-      <c r="C62" t="s">
-        <v>695</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -23647,6 +23659,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C67">
+    <sortCondition ref="B2:B67"/>
+  </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{A5789ACF-E5B3-4A72-A5A4-EFB9B8BB2DA2}">
       <formula1>"match, mismatch, unclear"</formula1>
@@ -23660,7 +23675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAB239F-5B5B-42C8-A8ED-88869190E609}">
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -24507,8 +24522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C72F94-F2BD-4B54-9CD8-146D4A928836}">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24537,23 +24552,23 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>278</v>
+        <v>729</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>729</v>
@@ -24561,23 +24576,23 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>729</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>729</v>
@@ -24585,7 +24600,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
         <v>729</v>
@@ -24593,7 +24608,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
         <v>729</v>
@@ -24601,7 +24616,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>729</v>
@@ -24609,7 +24624,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
         <v>729</v>
@@ -24617,23 +24632,26 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>278</v>
+        <v>729</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
         <v>729</v>
       </c>
+      <c r="C14" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
         <v>729</v>
@@ -24641,26 +24659,26 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="B17" t="s">
-        <v>278</v>
+        <v>729</v>
       </c>
       <c r="C17" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="B18" t="s">
         <v>729</v>
@@ -24668,7 +24686,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>585</v>
       </c>
       <c r="B19" t="s">
         <v>729</v>
@@ -24676,26 +24694,23 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>156</v>
       </c>
       <c r="B20" t="s">
-        <v>278</v>
+        <v>729</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="B21" t="s">
-        <v>278</v>
-      </c>
-      <c r="C21" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
         <v>729</v>
@@ -24703,37 +24718,31 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
       <c r="B23" t="s">
         <v>729</v>
       </c>
-      <c r="C23" t="s">
-        <v>733</v>
-      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>186</v>
       </c>
       <c r="B24" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
       <c r="B25" t="s">
-        <v>278</v>
-      </c>
-      <c r="C25" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
       <c r="B26" t="s">
         <v>729</v>
@@ -24741,15 +24750,15 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>208</v>
       </c>
       <c r="B27" t="s">
-        <v>278</v>
+        <v>729</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>217</v>
       </c>
       <c r="B28" t="s">
         <v>729</v>
@@ -24757,29 +24766,23 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>221</v>
       </c>
       <c r="B29" t="s">
         <v>729</v>
       </c>
-      <c r="C29" t="s">
-        <v>735</v>
-      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>225</v>
       </c>
       <c r="B30" t="s">
-        <v>278</v>
-      </c>
-      <c r="C30" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>147</v>
+        <v>229</v>
       </c>
       <c r="B31" t="s">
         <v>729</v>
@@ -24787,7 +24790,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>585</v>
+        <v>234</v>
       </c>
       <c r="B32" t="s">
         <v>729</v>
@@ -24795,7 +24798,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>239</v>
       </c>
       <c r="B33" t="s">
         <v>729</v>
@@ -24803,15 +24806,15 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>243</v>
       </c>
       <c r="B34" t="s">
-        <v>278</v>
+        <v>729</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>247</v>
       </c>
       <c r="B35" t="s">
         <v>729</v>
@@ -24819,7 +24822,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>169</v>
+        <v>252</v>
       </c>
       <c r="B36" t="s">
         <v>729</v>
@@ -24827,23 +24830,23 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>257</v>
       </c>
       <c r="B37" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>169</v>
+        <v>262</v>
       </c>
       <c r="B38" t="s">
-        <v>278</v>
+        <v>729</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>264</v>
       </c>
       <c r="B39" t="s">
         <v>729</v>
@@ -24851,23 +24854,23 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>179</v>
+        <v>267</v>
       </c>
       <c r="B40" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>182</v>
+        <v>269</v>
       </c>
       <c r="B41" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>186</v>
+        <v>275</v>
       </c>
       <c r="B42" t="s">
         <v>729</v>
@@ -24875,7 +24878,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>190</v>
+        <v>279</v>
       </c>
       <c r="B43" t="s">
         <v>729</v>
@@ -24883,23 +24886,23 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>190</v>
+        <v>283</v>
       </c>
       <c r="B44" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>193</v>
+        <v>286</v>
       </c>
       <c r="B45" t="s">
-        <v>278</v>
+        <v>729</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>198</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
         <v>730</v>
@@ -24907,69 +24910,66 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>204</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>208</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>278</v>
-      </c>
-      <c r="C49" t="s">
-        <v>737</v>
+        <v>730</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
       <c r="B50" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="B51" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="B52" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>229</v>
+        <v>190</v>
       </c>
       <c r="B53" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="B54" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -24982,117 +24982,135 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>239</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>729</v>
+        <v>278</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>243</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>729</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>247</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>729</v>
+        <v>278</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>249</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
         <v>278</v>
       </c>
+      <c r="C59" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>252</v>
+        <v>98</v>
       </c>
       <c r="B60" t="s">
-        <v>729</v>
+        <v>278</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>257</v>
+        <v>105</v>
       </c>
       <c r="B61" t="s">
-        <v>729</v>
+        <v>278</v>
+      </c>
+      <c r="C61" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>262</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>729</v>
+        <v>278</v>
+      </c>
+      <c r="C62" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>264</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>729</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>267</v>
+        <v>143</v>
       </c>
       <c r="B64" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="C64" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>269</v>
+        <v>162</v>
       </c>
       <c r="B65" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>275</v>
+        <v>169</v>
       </c>
       <c r="B66" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>279</v>
+        <v>193</v>
       </c>
       <c r="B67" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>283</v>
+        <v>213</v>
       </c>
       <c r="B68" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="C68" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>286</v>
+        <v>249</v>
       </c>
       <c r="B69" t="s">
-        <v>729</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C69">
+    <sortCondition ref="B1:B69"/>
+  </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{0BB362FB-DC38-48C2-A871-99AC57F9D5A8}">
       <formula1>"negative, positive, unclear"</formula1>

</xml_diff>